<commit_message>
1. Change in startup to stop tracking database changes. 2. Change in Blog for error related to tracking and implementation of security validation
</commit_message>
<xml_diff>
--- a/Blog Project Requirements - V1.1.xlsx
+++ b/Blog Project Requirements - V1.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sampe\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DABC9EA-0F60-4BAA-A047-0116DD0B9173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{809B1B41-5E81-4812-B0B7-44F981D57BC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3450" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{C699C9CA-C9B4-411F-AC3B-5900A1E1ED8E}"/>
+    <workbookView minimized="1" xWindow="11355" yWindow="-18690" windowWidth="21600" windowHeight="11295" xr2:uid="{C699C9CA-C9B4-411F-AC3B-5900A1E1ED8E}"/>
   </bookViews>
   <sheets>
     <sheet name="Blog Project Requirements" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="136">
   <si>
     <t>ID</t>
   </si>
@@ -437,6 +437,15 @@
   </si>
   <si>
     <t>ApplicationDbUser, Blog, Post, Comment, PostTag</t>
+  </si>
+  <si>
+    <t>DevOps</t>
+  </si>
+  <si>
+    <t>Git/Azure DevOps</t>
+  </si>
+  <si>
+    <t>Display Comment</t>
   </si>
 </sst>
 </file>
@@ -630,25 +639,22 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -663,17 +669,20 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1029,10 +1038,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{693F3315-BA5B-4142-ABE0-C43711898366}">
-  <dimension ref="A1:G125"/>
+  <dimension ref="A1:G126"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41:C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1048,23 +1057,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="16" t="s">
+      <c r="C1" s="24"/>
+      <c r="D1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="17" t="s">
         <v>124</v>
       </c>
     </row>
@@ -1091,6 +1100,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
+        <f>A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1112,13 +1122,14 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
+        <f t="shared" ref="A4:A8" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>49</v>
+        <v>133</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>44</v>
+        <v>134</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>4</v>
@@ -1127,61 +1138,64 @@
         <v>7</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>4</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>127</v>
+        <v>47</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>132</v>
+        <v>48</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>4</v>
@@ -1190,155 +1204,156 @@
         <v>7</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="3"/>
+      <c r="A8" s="3">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>125</v>
+      </c>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B10" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="C10" s="25"/>
+      <c r="D10" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B11" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C11" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:7" ht="33" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="D11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" ht="33" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B12" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C12" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
+      <c r="D12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>125</v>
+      </c>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B14" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-    </row>
-    <row r="14" spans="1:7" ht="33" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="G14" s="3"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:7" ht="33" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:7" ht="33" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B16" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C16" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>20</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>5</v>
@@ -1353,212 +1368,212 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B18" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C18" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="G17" s="3"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
+      <c r="D18" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>125</v>
+      </c>
       <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="3"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B20" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-    </row>
-    <row r="20" spans="1:7" ht="33" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="C20" s="26"/>
+      <c r="D20" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+    </row>
+    <row r="21" spans="1:7" ht="33" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B21" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C21" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="G20" s="3"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+      <c r="D21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B22" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C22" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="D21" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="G21" s="9"/>
-    </row>
-    <row r="22" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+      <c r="D22" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G22" s="9"/>
+    </row>
+    <row r="23" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B23" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C23" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D22" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="G22" s="9"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="G23" s="3"/>
+      <c r="D23" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G23" s="9"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="G24" s="3"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B25" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C25" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="G24" s="3"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
+      <c r="D25" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>125</v>
+      </c>
       <c r="G25" s="3"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="3"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B27" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="14"/>
-      <c r="D26" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-    </row>
-    <row r="27" spans="1:7" ht="33" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="C27" s="23"/>
+      <c r="D27" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+    </row>
+    <row r="28" spans="1:7" ht="33" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C28" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="G27" s="3"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>37</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>5</v>
@@ -1573,16 +1588,20 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
+        <v>37</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="F29" s="3" t="s">
         <v>125</v>
       </c>
@@ -1590,20 +1609,16 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>7</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
       <c r="F30" s="3" t="s">
         <v>125</v>
       </c>
@@ -1611,202 +1626,202 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="G31" s="3"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B32" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C32" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="G31" s="3"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
+      <c r="D32" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>125</v>
+      </c>
       <c r="G32" s="3"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
+      <c r="A33" s="3"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B33" s="13" t="s">
+      <c r="B34" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="C33" s="14"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-    </row>
-    <row r="34" spans="1:7" ht="33" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="G34" s="3"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
     </row>
     <row r="35" spans="1:7" ht="33" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="G35" s="3"/>
+    </row>
+    <row r="36" spans="1:7" ht="33" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B36" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C36" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="D35" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="G35" s="3"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="9" t="s">
+      <c r="D36" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="G36" s="3"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="B37" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="10" t="s">
+      <c r="C37" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D36" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="G36" s="3"/>
-    </row>
-    <row r="37" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+      <c r="D37" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="G37" s="3"/>
+    </row>
+    <row r="38" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B38" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C38" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="D37" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="G37" s="3"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="D38" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="G38" s="3"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B39" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C39" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="D38" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="G38" s="3"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
+      <c r="D39" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>125</v>
+      </c>
       <c r="G39" s="3"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B40" s="19" t="s">
+      <c r="B41" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="7"/>
-    </row>
-    <row r="41" spans="1:7" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+      <c r="C41" s="19"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+    </row>
+    <row r="42" spans="1:7" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B42" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C42" s="6" t="s">
         <v>108</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="G41" s="3"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>104</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>5</v>
@@ -1821,75 +1836,75 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="G43" s="3"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B44" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C44" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="G43" s="3"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
+      <c r="D44" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>125</v>
+      </c>
       <c r="G44" s="3"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="8" t="s">
+      <c r="A45" s="3"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B45" s="21" t="s">
+      <c r="B46" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="C45" s="22"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="7"/>
-    </row>
-    <row r="46" spans="1:7" ht="33" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
+      <c r="C46" s="21"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
+    </row>
+    <row r="47" spans="1:7" ht="33" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B46" s="3"/>
-      <c r="C46" s="6" t="s">
+      <c r="B47" s="3"/>
+      <c r="C47" s="6" t="s">
         <v>110</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="G46" s="3"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>121</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>5</v>
@@ -1904,178 +1919,182 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="G48" s="3"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B49" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="C49" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="D48" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F48" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="G48" s="3"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
+      <c r="D49" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>125</v>
+      </c>
       <c r="G49" s="3"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="8" t="s">
+      <c r="A50" s="3"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="B50" s="13" t="s">
+      <c r="B51" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="C50" s="14"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="7"/>
-      <c r="G50" s="7"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="B51" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="C51" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="D51" s="9"/>
-      <c r="E51" s="9"/>
-      <c r="F51" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="G51" s="3"/>
+      <c r="C51" s="23"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="7"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="B52" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="C52" s="23" t="s">
-        <v>39</v>
+        <v>115</v>
+      </c>
+      <c r="B52" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C52" s="14" t="s">
+        <v>116</v>
       </c>
       <c r="D52" s="9"/>
       <c r="E52" s="9"/>
       <c r="F52" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G52" s="3"/>
     </row>
-    <row r="53" spans="1:7" ht="165" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="B53" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="C53" s="23" t="s">
-        <v>129</v>
+        <v>117</v>
+      </c>
+      <c r="B53" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C53" s="14" t="s">
+        <v>39</v>
       </c>
       <c r="D53" s="9"/>
       <c r="E53" s="9"/>
       <c r="F53" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G53" s="3"/>
     </row>
-    <row r="54" spans="1:7" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
+    <row r="54" spans="1:7" ht="165" x14ac:dyDescent="0.3">
+      <c r="A54" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B54" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="G54" s="3"/>
+    </row>
+    <row r="55" spans="1:7" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B54" s="6" t="s">
+      <c r="B55" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C54" s="6" t="s">
+      <c r="C55" s="6" t="s">
         <v>122</v>
-      </c>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
-      <c r="G54" s="3"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C55" s="6" t="s">
-        <v>111</v>
       </c>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
-      <c r="F55" s="3" t="s">
-        <v>125</v>
-      </c>
+      <c r="F55" s="3"/>
       <c r="G55" s="3"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A56" s="3"/>
-      <c r="B56" s="24"/>
-      <c r="C56" s="25"/>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>111</v>
+      </c>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
-      <c r="F56" s="3"/>
+      <c r="F56" s="3" t="s">
+        <v>125</v>
+      </c>
       <c r="G56" s="3"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="8" t="s">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A57" s="3"/>
+      <c r="B57" s="15"/>
+      <c r="C57" s="16"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
+      <c r="G57" s="3"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B57" s="13" t="s">
+      <c r="B58" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C57" s="14"/>
-      <c r="D57" s="7"/>
-      <c r="E57" s="7"/>
-      <c r="F57" s="7"/>
-      <c r="G57" s="7"/>
-    </row>
-    <row r="58" spans="1:7" ht="33" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
+      <c r="C58" s="23"/>
+      <c r="D58" s="7"/>
+      <c r="E58" s="7"/>
+      <c r="F58" s="7"/>
+      <c r="G58" s="7"/>
+    </row>
+    <row r="59" spans="1:7" ht="33" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B59" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C58" s="6" t="s">
+      <c r="C59" s="6" t="s">
         <v>80</v>
-      </c>
-      <c r="D58" s="3"/>
-      <c r="E58" s="3"/>
-      <c r="F58" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="G58" s="3"/>
-    </row>
-    <row r="59" spans="1:7" ht="82.5" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="C59" s="6" t="s">
-        <v>9</v>
       </c>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
@@ -2084,15 +2103,15 @@
       </c>
       <c r="G59" s="3"/>
     </row>
-    <row r="60" spans="1:7" ht="33" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="82.5" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
@@ -2101,13 +2120,15 @@
       </c>
       <c r="G60" s="3"/>
     </row>
-    <row r="61" spans="1:7" ht="66" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" ht="33" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B61" s="3"/>
+        <v>83</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>130</v>
+      </c>
       <c r="C61" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
@@ -2118,13 +2139,13 @@
     </row>
     <row r="62" spans="1:7" ht="66" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>91</v>
+        <v>135</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>92</v>
+        <v>11</v>
       </c>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
@@ -2133,15 +2154,15 @@
       </c>
       <c r="G62" s="3"/>
     </row>
-    <row r="63" spans="1:7" ht="33" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="66" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
@@ -2150,15 +2171,15 @@
       </c>
       <c r="G63" s="3"/>
     </row>
-    <row r="64" spans="1:7" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" ht="33" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>15</v>
+        <v>89</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
@@ -2167,13 +2188,21 @@
       </c>
       <c r="G64" s="3"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="3"/>
-      <c r="B65" s="3"/>
-      <c r="C65" s="6"/>
+    <row r="65" spans="1:7" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>88</v>
+      </c>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
-      <c r="F65" s="3"/>
+      <c r="F65" s="3" t="s">
+        <v>125</v>
+      </c>
       <c r="G65" s="3"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -2716,18 +2745,27 @@
       <c r="F125" s="3"/>
       <c r="G125" s="3"/>
     </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A126" s="3"/>
+      <c r="B126" s="3"/>
+      <c r="C126" s="6"/>
+      <c r="D126" s="3"/>
+      <c r="E126" s="3"/>
+      <c r="F126" s="3"/>
+      <c r="G126" s="3"/>
+    </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B58:C58"/>
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B34:C34"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>